<commit_message>
[CORE] Multi-Core Boot Verified
</commit_message>
<xml_diff>
--- a/documentation/RP5_Peripheral_Register_Map.xlsx
+++ b/documentation/RP5_Peripheral_Register_Map.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QEMU_Cortex-A72\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D465B882-628E-46CA-8631-1060F740B595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete_Register_Map" sheetId="1" r:id="rId1"/>
@@ -13,7 +19,7 @@
     <sheet name="Atomic_Access" sheetId="4" r:id="rId4"/>
     <sheet name="Interrupt_Modes" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1025,8 +1031,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1035,12 +1041,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1055,14 +1067,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1109,7 +1130,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1141,9 +1162,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1175,6 +1214,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1350,42 +1407,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1405,7 +1464,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1484,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1504,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1465,7 +1524,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1485,7 +1544,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1505,7 +1564,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1525,7 +1584,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1545,7 +1604,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1565,7 +1624,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1585,7 +1644,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1605,7 +1664,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1625,7 +1684,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1645,7 +1704,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1665,7 +1724,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1685,7 +1744,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1705,7 +1764,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1725,7 +1784,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1745,7 +1804,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1765,7 +1824,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1785,7 +1844,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1805,7 +1864,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1825,7 +1884,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1845,7 +1904,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1865,7 +1924,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1885,7 +1944,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1905,7 +1964,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1925,7 +1984,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1945,7 +2004,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1965,7 +2024,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1985,7 +2044,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2005,7 +2064,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2025,7 +2084,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -2045,7 +2104,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2065,7 +2124,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -2085,7 +2144,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -2105,7 +2164,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -2125,7 +2184,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -2145,7 +2204,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -2165,7 +2224,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -2185,7 +2244,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -2205,7 +2264,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -2225,7 +2284,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -2245,7 +2304,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -2265,7 +2324,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -2285,7 +2344,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -2305,7 +2364,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -2325,7 +2384,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -2345,7 +2404,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -2365,7 +2424,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -2385,7 +2444,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -2405,7 +2464,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -2425,7 +2484,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2451,33 +2510,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>192</v>
       </c>
@@ -2491,7 +2552,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>193</v>
       </c>
@@ -2505,7 +2566,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -2519,7 +2580,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -2533,7 +2594,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>196</v>
       </c>
@@ -2547,7 +2608,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -2561,7 +2622,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>198</v>
       </c>
@@ -2575,7 +2636,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>199</v>
       </c>
@@ -2589,7 +2650,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>200</v>
       </c>
@@ -2603,7 +2664,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>201</v>
       </c>
@@ -2617,7 +2678,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>202</v>
       </c>
@@ -2631,7 +2692,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>203</v>
       </c>
@@ -2645,7 +2706,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>204</v>
       </c>
@@ -2659,7 +2720,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>205</v>
       </c>
@@ -2673,7 +2734,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>206</v>
       </c>
@@ -2687,7 +2748,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>207</v>
       </c>
@@ -2701,7 +2762,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>208</v>
       </c>
@@ -2721,33 +2782,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>247</v>
       </c>
@@ -2761,7 +2824,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>248</v>
       </c>
@@ -2775,7 +2838,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>249</v>
       </c>
@@ -2789,7 +2852,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>250</v>
       </c>
@@ -2803,7 +2866,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>251</v>
       </c>
@@ -2817,7 +2880,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>252</v>
       </c>
@@ -2831,7 +2894,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -2845,7 +2908,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>254</v>
       </c>
@@ -2859,7 +2922,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>255</v>
       </c>
@@ -2873,7 +2936,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>256</v>
       </c>
@@ -2887,7 +2950,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>257</v>
       </c>
@@ -2901,7 +2964,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>258</v>
       </c>
@@ -2921,30 +2984,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>284</v>
       </c>
@@ -2955,7 +3020,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>285</v>
       </c>
@@ -2966,7 +3031,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>286</v>
       </c>
@@ -2977,7 +3042,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>287</v>
       </c>
@@ -2988,12 +3053,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3004,7 +3069,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>289</v>
       </c>
@@ -3015,7 +3080,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>290</v>
       </c>
@@ -3026,7 +3091,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>291</v>
       </c>
@@ -3037,7 +3102,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>292</v>
       </c>
@@ -3051,29 +3116,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="1" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>308</v>
       </c>
@@ -3084,7 +3151,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>309</v>
       </c>
@@ -3095,7 +3162,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>310</v>
       </c>
@@ -3106,7 +3173,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>311</v>
       </c>
@@ -3117,7 +3184,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -3128,7 +3195,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>313</v>
       </c>
@@ -3139,7 +3206,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>314</v>
       </c>
@@ -3150,7 +3217,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>315</v>
       </c>

</xml_diff>